<commit_message>
empieza test de la ia
</commit_message>
<xml_diff>
--- a/back/datos.xlsx
+++ b/back/datos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,32 +421,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>Segundo</v>
+        <v>primer</v>
       </c>
       <c r="C2" t="str">
-        <v>pase</v>
+        <v>kickoff</v>
       </c>
       <c r="D2" t="str">
-        <v>-2'</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Segundo</v>
-      </c>
-      <c r="C3" t="str">
-        <v>pase</v>
-      </c>
-      <c r="D3" t="str">
-        <v>+8'</v>
+        <v>37'</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Conexion entre frontend y backend exitosa
</commit_message>
<xml_diff>
--- a/back/datos.xlsx
+++ b/back/datos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,32 +421,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>Segundo</v>
+        <v>Down (primero</v>
       </c>
       <c r="C2" t="str">
-        <v>pase</v>
+        <v>segundo</v>
       </c>
       <c r="D2" t="str">
-        <v>-2'</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Segundo</v>
-      </c>
-      <c r="C3" t="str">
-        <v>pase</v>
-      </c>
-      <c r="D3" t="str">
-        <v>+8'</v>
+        <v>tercero</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se saco la base de datos de notion, aunque se conserva el código
</commit_message>
<xml_diff>
--- a/back/datos.xlsx
+++ b/back/datos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,23 +416,39 @@
         <v>Yardas G/P</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" xml:space="preserve">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="str">
-        <v>Down (primero</v>
+      <c r="B2" t="str" xml:space="preserve">
+        <v xml:space="preserve">``json
+[
+  "Down (primer</v>
       </c>
       <c r="C2" t="str">
         <v>segundo</v>
       </c>
       <c r="D2" t="str">
         <v>tercero</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Primero</v>
+      </c>
+      <c r="C3" t="str">
+        <v>pase</v>
+      </c>
+      <c r="D3" t="str">
+        <v>15'</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se agrego variable de entorno y prueba
</commit_message>
<xml_diff>
--- a/back/datos.xlsx
+++ b/back/datos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,23 +416,9 @@
         <v>Yardas G/P</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <v>primer</v>
-      </c>
-      <c r="C2" t="str">
-        <v>kickoff</v>
-      </c>
-      <c r="D2" t="str">
-        <v>37'</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>